<commit_message>
Complete Project plan document, add Testing plan dpcument
</commit_message>
<xml_diff>
--- a/Document/ke hoach thuc hien .xlsx
+++ b/Document/ke hoach thuc hien .xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Tên đồ án:</t>
   </si>
@@ -79,10 +79,6 @@
   </si>
   <si>
     <t>VIDEO RENTAL STORE SYSTEM</t>
-  </si>
-  <si>
-    <t>Tạo sơ đồ thực thể, sơ đồ thực thể quan hệ, sơ đồ lớp, view flow - Team
-Phân tích usecase, vẽ lược đồ trình tự (sequence diagram) và lược đồ hoạt động (activity diagram), lập bảng Test-case - Theo usecase được phân công</t>
   </si>
   <si>
     <t>Phân tích yêu cầu và lập usecase tổng quát - Team
@@ -90,9 +86,32 @@
 Tạo project repository trên Github - Nguyễn Thanh Nga</t>
   </si>
   <si>
+    <t>Coding - Theo usecase được phân công</t>
+  </si>
+  <si>
+    <t>Báo cáo đề tài, triển khai hệ thống - Team</t>
+  </si>
+  <si>
+    <t>Tiến hành kiểm thử chức năng, hiệu chỉnh - Theo usecase được phân công</t>
+  </si>
+  <si>
+    <t>Kiểm thử tích hợp , hiệu chỉnh - Team</t>
+  </si>
+  <si>
+    <t>Kiểm thử hệ thống, hiệu chỉnh,  lập tài liệu hướng dẫn sử dụng - Team</t>
+  </si>
+  <si>
+    <t>Kiểm thử hệ thống, hiệu chỉnh - Team</t>
+  </si>
+  <si>
     <t>Tạo khung project, tạo database - Nguyễn Thanh Nga
 Thảo luận, hoàn thiện các lược đồ - Team
-Vẽ mockup cho các view - Theo usecase được phân công</t>
+Vẽ mockup cho các view,  lập bảng Test-case - Theo usecase được phân công</t>
+  </si>
+  <si>
+    <t>Tạo sơ đồ thực thể, sơ đồ thực thể quan hệ, sơ đồ lớp, view flow - Team
+Phân tích usecase, vẽ lược đồ trình tự (sequence diagram) và lược đồ hoạt động (activity diagram) - Theo usecase được phân công
+Lập kế hoạch kiểm thử - Nguyễn Thanh Nga</t>
   </si>
 </sst>
 </file>
@@ -102,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +195,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -269,7 +294,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -326,12 +351,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,7 +364,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -623,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.77734375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -676,7 +704,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6">
-        <v>42802</v>
+        <v>42950</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -702,14 +730,14 @@
       </c>
       <c r="B6" s="11">
         <f>C4</f>
-        <v>42802</v>
+        <v>42950</v>
       </c>
       <c r="C6" s="19">
         <f>B6+6</f>
-        <v>42808</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>11</v>
+        <v>42956</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="E6" s="17"/>
     </row>
@@ -719,30 +747,30 @@
       </c>
       <c r="B7" s="11">
         <f>B6+7</f>
-        <v>42809</v>
+        <v>42957</v>
       </c>
       <c r="C7" s="20">
         <f t="shared" ref="C7:C20" si="0">B7+6</f>
-        <v>42815</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+        <v>42963</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>3</v>
       </c>
       <c r="B8" s="11">
         <f t="shared" ref="B8:B20" si="1">B7+7</f>
-        <v>42816</v>
+        <v>42964</v>
       </c>
       <c r="C8" s="20">
         <f t="shared" si="0"/>
-        <v>42822</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>12</v>
+        <v>42970</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -751,13 +779,15 @@
       </c>
       <c r="B9" s="11">
         <f t="shared" si="1"/>
-        <v>42823</v>
+        <v>42971</v>
       </c>
       <c r="C9" s="20">
         <f t="shared" si="0"/>
-        <v>42829</v>
-      </c>
-      <c r="D9" s="22"/>
+        <v>42977</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
@@ -765,13 +795,15 @@
       </c>
       <c r="B10" s="11">
         <f t="shared" si="1"/>
-        <v>42830</v>
+        <v>42978</v>
       </c>
       <c r="C10" s="20">
         <f t="shared" si="0"/>
-        <v>42836</v>
-      </c>
-      <c r="D10" s="22"/>
+        <v>42984</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
@@ -779,13 +811,15 @@
       </c>
       <c r="B11" s="11">
         <f t="shared" si="1"/>
-        <v>42837</v>
+        <v>42985</v>
       </c>
       <c r="C11" s="20">
         <f t="shared" si="0"/>
-        <v>42843</v>
-      </c>
-      <c r="D11" s="22"/>
+        <v>42991</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
@@ -793,13 +827,15 @@
       </c>
       <c r="B12" s="11">
         <f t="shared" si="1"/>
-        <v>42844</v>
+        <v>42992</v>
       </c>
       <c r="C12" s="20">
         <f t="shared" si="0"/>
-        <v>42850</v>
-      </c>
-      <c r="D12" s="22"/>
+        <v>42998</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
@@ -807,13 +843,15 @@
       </c>
       <c r="B13" s="11">
         <f t="shared" si="1"/>
-        <v>42851</v>
+        <v>42999</v>
       </c>
       <c r="C13" s="20">
         <f t="shared" si="0"/>
-        <v>42857</v>
-      </c>
-      <c r="D13" s="22"/>
+        <v>43005</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
@@ -821,13 +859,15 @@
       </c>
       <c r="B14" s="11">
         <f t="shared" si="1"/>
-        <v>42858</v>
+        <v>43006</v>
       </c>
       <c r="C14" s="20">
         <f t="shared" si="0"/>
-        <v>42864</v>
-      </c>
-      <c r="D14" s="22"/>
+        <v>43012</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
@@ -835,13 +875,15 @@
       </c>
       <c r="B15" s="11">
         <f t="shared" si="1"/>
-        <v>42865</v>
+        <v>43013</v>
       </c>
       <c r="C15" s="20">
         <f t="shared" si="0"/>
-        <v>42871</v>
-      </c>
-      <c r="D15" s="22"/>
+        <v>43019</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
@@ -849,13 +891,15 @@
       </c>
       <c r="B16" s="11">
         <f t="shared" si="1"/>
-        <v>42872</v>
+        <v>43020</v>
       </c>
       <c r="C16" s="20">
         <f t="shared" si="0"/>
-        <v>42878</v>
-      </c>
-      <c r="D16" s="22"/>
+        <v>43026</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
@@ -863,13 +907,15 @@
       </c>
       <c r="B17" s="11">
         <f t="shared" si="1"/>
-        <v>42879</v>
+        <v>43027</v>
       </c>
       <c r="C17" s="20">
         <f t="shared" si="0"/>
-        <v>42885</v>
-      </c>
-      <c r="D17" s="22"/>
+        <v>43033</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
@@ -877,13 +923,15 @@
       </c>
       <c r="B18" s="11">
         <f t="shared" si="1"/>
-        <v>42886</v>
+        <v>43034</v>
       </c>
       <c r="C18" s="20">
         <f t="shared" si="0"/>
-        <v>42892</v>
-      </c>
-      <c r="D18" s="22"/>
+        <v>43040</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
@@ -891,13 +939,15 @@
       </c>
       <c r="B19" s="11">
         <f t="shared" si="1"/>
-        <v>42893</v>
+        <v>43041</v>
       </c>
       <c r="C19" s="20">
         <f t="shared" si="0"/>
-        <v>42899</v>
-      </c>
-      <c r="D19" s="22"/>
+        <v>43047</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
@@ -905,13 +955,18 @@
       </c>
       <c r="B20" s="11">
         <f t="shared" si="1"/>
-        <v>42900</v>
+        <v>43048</v>
       </c>
       <c r="C20" s="20">
         <f t="shared" si="0"/>
-        <v>42906</v>
-      </c>
-      <c r="D20" s="22"/>
+        <v>43054</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
add dac ta phi
</commit_message>
<xml_diff>
--- a/Document/ke hoach thuc hien .xlsx
+++ b/Document/ke hoach thuc hien .xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Tên đồ án:</t>
   </si>
@@ -79,10 +79,6 @@
   </si>
   <si>
     <t>VIDEO RENTAL STORE SYSTEM</t>
-  </si>
-  <si>
-    <t>Tạo sơ đồ thực thể, sơ đồ thực thể quan hệ, sơ đồ lớp, view flow - Team
-Phân tích usecase, vẽ lược đồ trình tự (sequence diagram) và lược đồ hoạt động (activity diagram), lập bảng Test-case - Theo usecase được phân công</t>
   </si>
   <si>
     <t>Phân tích yêu cầu và lập usecase tổng quát - Team
@@ -90,9 +86,32 @@
 Tạo project repository trên Github - Nguyễn Thanh Nga</t>
   </si>
   <si>
+    <t>Coding - Theo usecase được phân công</t>
+  </si>
+  <si>
+    <t>Báo cáo đề tài, triển khai hệ thống - Team</t>
+  </si>
+  <si>
+    <t>Tiến hành kiểm thử chức năng, hiệu chỉnh - Theo usecase được phân công</t>
+  </si>
+  <si>
+    <t>Kiểm thử tích hợp , hiệu chỉnh - Team</t>
+  </si>
+  <si>
+    <t>Kiểm thử hệ thống, hiệu chỉnh,  lập tài liệu hướng dẫn sử dụng - Team</t>
+  </si>
+  <si>
+    <t>Kiểm thử hệ thống, hiệu chỉnh - Team</t>
+  </si>
+  <si>
     <t>Tạo khung project, tạo database - Nguyễn Thanh Nga
 Thảo luận, hoàn thiện các lược đồ - Team
-Vẽ mockup cho các view - Theo usecase được phân công</t>
+Vẽ mockup cho các view,  lập bảng Test-case - Theo usecase được phân công</t>
+  </si>
+  <si>
+    <t>Tạo sơ đồ thực thể, sơ đồ thực thể quan hệ, sơ đồ lớp, view flow - Team
+Phân tích usecase, vẽ lược đồ trình tự (sequence diagram) và lược đồ hoạt động (activity diagram) - Theo usecase được phân công
+Lập kế hoạch kiểm thử - Nguyễn Thanh Nga</t>
   </si>
 </sst>
 </file>
@@ -102,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +195,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -269,7 +294,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -326,12 +351,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,7 +364,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -623,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.77734375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -676,7 +704,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6">
-        <v>42802</v>
+        <v>42950</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -702,14 +730,14 @@
       </c>
       <c r="B6" s="11">
         <f>C4</f>
-        <v>42802</v>
+        <v>42950</v>
       </c>
       <c r="C6" s="19">
         <f>B6+6</f>
-        <v>42808</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>11</v>
+        <v>42956</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="E6" s="17"/>
     </row>
@@ -719,30 +747,30 @@
       </c>
       <c r="B7" s="11">
         <f>B6+7</f>
-        <v>42809</v>
+        <v>42957</v>
       </c>
       <c r="C7" s="20">
         <f t="shared" ref="C7:C20" si="0">B7+6</f>
-        <v>42815</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+        <v>42963</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>3</v>
       </c>
       <c r="B8" s="11">
         <f t="shared" ref="B8:B20" si="1">B7+7</f>
-        <v>42816</v>
+        <v>42964</v>
       </c>
       <c r="C8" s="20">
         <f t="shared" si="0"/>
-        <v>42822</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>12</v>
+        <v>42970</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -751,13 +779,15 @@
       </c>
       <c r="B9" s="11">
         <f t="shared" si="1"/>
-        <v>42823</v>
+        <v>42971</v>
       </c>
       <c r="C9" s="20">
         <f t="shared" si="0"/>
-        <v>42829</v>
-      </c>
-      <c r="D9" s="22"/>
+        <v>42977</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
@@ -765,13 +795,15 @@
       </c>
       <c r="B10" s="11">
         <f t="shared" si="1"/>
-        <v>42830</v>
+        <v>42978</v>
       </c>
       <c r="C10" s="20">
         <f t="shared" si="0"/>
-        <v>42836</v>
-      </c>
-      <c r="D10" s="22"/>
+        <v>42984</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
@@ -779,13 +811,15 @@
       </c>
       <c r="B11" s="11">
         <f t="shared" si="1"/>
-        <v>42837</v>
+        <v>42985</v>
       </c>
       <c r="C11" s="20">
         <f t="shared" si="0"/>
-        <v>42843</v>
-      </c>
-      <c r="D11" s="22"/>
+        <v>42991</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
@@ -793,13 +827,15 @@
       </c>
       <c r="B12" s="11">
         <f t="shared" si="1"/>
-        <v>42844</v>
+        <v>42992</v>
       </c>
       <c r="C12" s="20">
         <f t="shared" si="0"/>
-        <v>42850</v>
-      </c>
-      <c r="D12" s="22"/>
+        <v>42998</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
@@ -807,13 +843,15 @@
       </c>
       <c r="B13" s="11">
         <f t="shared" si="1"/>
-        <v>42851</v>
+        <v>42999</v>
       </c>
       <c r="C13" s="20">
         <f t="shared" si="0"/>
-        <v>42857</v>
-      </c>
-      <c r="D13" s="22"/>
+        <v>43005</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
@@ -821,13 +859,15 @@
       </c>
       <c r="B14" s="11">
         <f t="shared" si="1"/>
-        <v>42858</v>
+        <v>43006</v>
       </c>
       <c r="C14" s="20">
         <f t="shared" si="0"/>
-        <v>42864</v>
-      </c>
-      <c r="D14" s="22"/>
+        <v>43012</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
@@ -835,13 +875,15 @@
       </c>
       <c r="B15" s="11">
         <f t="shared" si="1"/>
-        <v>42865</v>
+        <v>43013</v>
       </c>
       <c r="C15" s="20">
         <f t="shared" si="0"/>
-        <v>42871</v>
-      </c>
-      <c r="D15" s="22"/>
+        <v>43019</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
@@ -849,13 +891,15 @@
       </c>
       <c r="B16" s="11">
         <f t="shared" si="1"/>
-        <v>42872</v>
+        <v>43020</v>
       </c>
       <c r="C16" s="20">
         <f t="shared" si="0"/>
-        <v>42878</v>
-      </c>
-      <c r="D16" s="22"/>
+        <v>43026</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
@@ -863,13 +907,15 @@
       </c>
       <c r="B17" s="11">
         <f t="shared" si="1"/>
-        <v>42879</v>
+        <v>43027</v>
       </c>
       <c r="C17" s="20">
         <f t="shared" si="0"/>
-        <v>42885</v>
-      </c>
-      <c r="D17" s="22"/>
+        <v>43033</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
@@ -877,13 +923,15 @@
       </c>
       <c r="B18" s="11">
         <f t="shared" si="1"/>
-        <v>42886</v>
+        <v>43034</v>
       </c>
       <c r="C18" s="20">
         <f t="shared" si="0"/>
-        <v>42892</v>
-      </c>
-      <c r="D18" s="22"/>
+        <v>43040</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
@@ -891,13 +939,15 @@
       </c>
       <c r="B19" s="11">
         <f t="shared" si="1"/>
-        <v>42893</v>
+        <v>43041</v>
       </c>
       <c r="C19" s="20">
         <f t="shared" si="0"/>
-        <v>42899</v>
-      </c>
-      <c r="D19" s="22"/>
+        <v>43047</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
@@ -905,13 +955,18 @@
       </c>
       <c r="B20" s="11">
         <f t="shared" si="1"/>
-        <v>42900</v>
+        <v>43048</v>
       </c>
       <c r="C20" s="20">
         <f t="shared" si="0"/>
-        <v>42906</v>
-      </c>
-      <c r="D20" s="22"/>
+        <v>43054</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>